<commit_message>
viettx day code 20170920
</commit_message>
<xml_diff>
--- a/CKPManagement/src/main/webapp/file/export/error/error_pumps_data.xlsx
+++ b/CKPManagement/src/main/webapp/file/export/error/error_pumps_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>C«ng ty cæ phÇn ckp</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>${data_JxLsC_.description}</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>B00100</t>
@@ -659,24 +656,26 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="8" t="n">
+        <v>1.0</v>
+      </c>
       <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>